<commit_message>
Validación en booking fecha
</commit_message>
<xml_diff>
--- a/Assets/docs/Trimestre II/03_Requisitos/historias de usuario.xlsx
+++ b/Assets/docs/Trimestre II/03_Requisitos/historias de usuario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aeoleco-my.sharepoint.com/personal/jvaron_aeole_co/Documents/Documentos/prueba/conjuntos_residenciales-main/Assets/docs/Trimestre II/03_Requisitos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\conjuntos_residenciales-main\Assets\docs\Trimestre II\03_Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{0368FBCC-4A0C-4971-B5D6-AD8EBC0B2A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB0C95A4-4988-4C7A-98A6-BC3D38262088}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4504DD55-BDDA-47D1-AC1D-1F39623A302C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lla de historia de usuario ágil" sheetId="1" r:id="rId1"/>
@@ -77,12 +77,6 @@
     <t>los habitantes quieren que el modulo para reservar el salon comunal sea facil de entender y claro con los datos que se toman. Esto para que sea mucho mas claros los motivos y la cantidad de asistentes en el evento. Igualmente que esten claras las medidas de seguridad a tener en cuenta</t>
   </si>
   <si>
-    <t>funcionalidades reserva parqueadero</t>
-  </si>
-  <si>
-    <t>los habirantes quieren que la reserva de este se pueda hacer por medio de la pagina web, para poder agilizar las visitas al conjunto. Esto les beneficia para poder agendar un parqueadero por cierto tiempo o simplemente para tenerlo a disposicion en una emergencia. Igualmente. El vigilante que se encuentre en turno, podra registrar tambien la ocupacion de un parqueadero</t>
-  </si>
-  <si>
     <t>colores</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>los habitantes piden que cunado hayan eventos especiales como asambleas, reuniones etc, se registren en la zona de eventos y los parqueaderos queden ocupados, puesto que en este lugar(casi siempre) es el espacio que se usa para hacer este tipo de eventos</t>
+  </si>
+  <si>
+    <t>modelo responsive</t>
+  </si>
+  <si>
+    <t>los habitantes pidieron que la pagina funcione lo mejor posible tanto en celular como en un computador</t>
   </si>
 </sst>
 </file>
@@ -738,27 +738,27 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="24.25" customWidth="1"/>
-    <col min="4" max="5" width="48.75" customWidth="1"/>
-    <col min="6" max="6" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" customWidth="1"/>
+    <col min="3" max="3" width="24.19921875" customWidth="1"/>
+    <col min="4" max="5" width="48.69921875" customWidth="1"/>
+    <col min="6" max="6" width="3.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
@@ -780,7 +780,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -796,7 +796,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -818,7 +818,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -862,7 +862,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -870,10 +870,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -884,7 +884,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -892,10 +892,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -906,7 +906,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -914,10 +914,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -928,7 +928,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -958,10 +958,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -972,7 +972,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -980,10 +980,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -994,7 +994,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -1002,10 +1002,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1016,7 +1016,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -1024,10 +1024,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1038,7 +1038,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -1046,10 +1046,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1060,7 +1060,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>14</v>
       </c>
@@ -1068,10 +1068,10 @@
         <v>7</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1082,7 +1082,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12">
         <v>15</v>
       </c>
@@ -1090,10 +1090,10 @@
         <v>8</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1104,7 +1104,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>16</v>
       </c>
@@ -1112,10 +1112,10 @@
         <v>8</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1126,7 +1126,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
@@ -1140,7 +1140,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="14"/>
@@ -1154,7 +1154,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="16"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18"/>
@@ -1168,7 +1168,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="2:13" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1182,7 +1182,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="2:13" s="11" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" s="11" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="20" t="s">
         <v>5</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1204,7 +1204,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1218,7 +1218,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1232,7 +1232,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1246,7 +1246,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1260,7 +1260,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1274,7 +1274,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1288,7 +1288,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1302,7 +1302,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1316,7 +1316,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1330,7 +1330,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1344,7 +1344,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1358,7 +1358,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1372,7 +1372,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1386,7 +1386,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1400,7 +1400,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1414,7 +1414,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1428,7 +1428,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1442,7 +1442,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1456,7 +1456,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1470,7 +1470,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1484,7 +1484,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1498,7 +1498,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1512,7 +1512,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1526,7 +1526,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1540,7 +1540,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1554,7 +1554,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1568,7 +1568,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1582,7 +1582,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1596,7 +1596,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1610,7 +1610,7 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1624,7 +1624,7 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1638,7 +1638,7 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1652,7 +1652,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1666,7 +1666,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1680,7 +1680,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1694,7 +1694,7 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1708,7 +1708,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -1722,7 +1722,7 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -1736,7 +1736,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -1750,7 +1750,7 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -1764,7 +1764,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -1778,7 +1778,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -1811,15 +1811,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="88.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.75" style="2"/>
+    <col min="1" max="1" width="3.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="88.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.69921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>